<commit_message>
Add oil tariffs to script
</commit_message>
<xml_diff>
--- a/lib/btap/measures/UtilityTariffs/resources/utility_tariffs.xlsx
+++ b/lib/btap/measures/UtilityTariffs/resources/utility_tariffs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="19440" windowHeight="11580" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="19440" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="utility_electricity_tariffs" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="158">
   <si>
     <t>Utility</t>
   </si>
@@ -480,10 +480,16 @@
     <t>Delivery</t>
   </si>
   <si>
-    <t>None</t>
+    <t>Manitoba</t>
   </si>
   <si>
-    <t>Manitoba</t>
+    <t>Centra</t>
+  </si>
+  <si>
+    <t>NoneGas</t>
+  </si>
+  <si>
+    <t>NoneOil</t>
   </si>
 </sst>
 </file>
@@ -833,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C80"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6311,13 +6317,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V80"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
@@ -9129,13 +9135,13 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="B42" t="s">
         <v>110</v>
       </c>
       <c r="C42" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D42">
         <v>14</v>
@@ -9197,13 +9203,13 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
         <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D43">
         <v>14</v>
@@ -9265,7 +9271,7 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B44" t="s">
         <v>85</v>
@@ -9333,7 +9339,7 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B45" t="s">
         <v>93</v>
@@ -9401,13 +9407,13 @@
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B46" t="s">
         <v>109</v>
       </c>
       <c r="C46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -9469,7 +9475,7 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B47" t="s">
         <v>82</v>
@@ -9537,7 +9543,7 @@
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B48" t="s">
         <v>84</v>
@@ -9605,7 +9611,7 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B49" t="s">
         <v>70</v>
@@ -9673,7 +9679,7 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B50" t="s">
         <v>135</v>
@@ -9741,7 +9747,7 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B51" t="s">
         <v>63</v>
@@ -9809,7 +9815,7 @@
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B52" t="s">
         <v>76</v>
@@ -9877,7 +9883,7 @@
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B53" t="s">
         <v>71</v>
@@ -9945,7 +9951,7 @@
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B54" t="s">
         <v>61</v>
@@ -10013,7 +10019,7 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B55" t="s">
         <v>64</v>
@@ -10081,7 +10087,7 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B56" t="s">
         <v>69</v>
@@ -10149,7 +10155,7 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B57" t="s">
         <v>136</v>
@@ -10217,7 +10223,7 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B58" t="s">
         <v>57</v>
@@ -10285,7 +10291,7 @@
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B59" t="s">
         <v>62</v>
@@ -10353,7 +10359,7 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B60" t="s">
         <v>68</v>
@@ -10421,7 +10427,7 @@
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B61" t="s">
         <v>80</v>
@@ -10489,7 +10495,7 @@
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B62" t="s">
         <v>83</v>
@@ -10557,7 +10563,7 @@
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B63" t="s">
         <v>91</v>
@@ -10625,13 +10631,13 @@
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B64" t="s">
         <v>107</v>
       </c>
       <c r="C64" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -10693,7 +10699,7 @@
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B65" t="s">
         <v>90</v>
@@ -10761,7 +10767,7 @@
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B66" t="s">
         <v>75</v>
@@ -10829,7 +10835,7 @@
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B67" t="s">
         <v>130</v>
@@ -11791,14 +11797,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V77" sqref="V77"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
@@ -13521,7 +13527,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B26" t="s">
         <v>121</v>
@@ -13589,7 +13595,7 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B27" t="s">
         <v>67</v>
@@ -13657,7 +13663,7 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B28" t="s">
         <v>66</v>
@@ -13725,7 +13731,7 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
         <v>110</v>
@@ -13793,7 +13799,7 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B30" t="s">
         <v>118</v>
@@ -13861,7 +13867,7 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B31" t="s">
         <v>128</v>
@@ -13929,7 +13935,7 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B32" t="s">
         <v>123</v>
@@ -13997,7 +14003,7 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B33" t="s">
         <v>120</v>
@@ -14065,7 +14071,7 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B34" t="s">
         <v>111</v>
@@ -14133,7 +14139,7 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B35" t="s">
         <v>115</v>
@@ -14201,7 +14207,7 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B36" t="s">
         <v>132</v>
@@ -14269,7 +14275,7 @@
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B37" t="s">
         <v>87</v>
@@ -14337,7 +14343,7 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B38" t="s">
         <v>116</v>
@@ -14405,7 +14411,7 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B39" t="s">
         <v>89</v>
@@ -14473,7 +14479,7 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B40" t="s">
         <v>129</v>
@@ -14541,7 +14547,7 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B41" t="s">
         <v>100</v>
@@ -14609,7 +14615,7 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B42" t="s">
         <v>117</v>
@@ -14677,7 +14683,7 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B43" t="s">
         <v>98</v>
@@ -14745,7 +14751,7 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B44" t="s">
         <v>119</v>
@@ -14813,7 +14819,7 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B45" t="s">
         <v>88</v>
@@ -14881,7 +14887,7 @@
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B46" t="s">
         <v>59</v>
@@ -14949,7 +14955,7 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B47" t="s">
         <v>72</v>
@@ -15017,7 +15023,7 @@
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B48" t="s">
         <v>74</v>
@@ -15085,7 +15091,7 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B49" t="s">
         <v>101</v>
@@ -15153,7 +15159,7 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B50" t="s">
         <v>102</v>
@@ -15221,7 +15227,7 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B51" t="s">
         <v>112</v>
@@ -15289,7 +15295,7 @@
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B52" t="s">
         <v>96</v>
@@ -15357,7 +15363,7 @@
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B53" t="s">
         <v>94</v>
@@ -15425,7 +15431,7 @@
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B54" t="s">
         <v>126</v>
@@ -15493,7 +15499,7 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B55" t="s">
         <v>133</v>
@@ -15561,7 +15567,7 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B56" t="s">
         <v>131</v>
@@ -15629,7 +15635,7 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B57" t="s">
         <v>56</v>
@@ -15697,7 +15703,7 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B58" t="s">
         <v>79</v>
@@ -15765,7 +15771,7 @@
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B59" t="s">
         <v>65</v>
@@ -15833,7 +15839,7 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B60" t="s">
         <v>55</v>
@@ -15901,7 +15907,7 @@
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B61" t="s">
         <v>86</v>
@@ -15969,7 +15975,7 @@
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B62" t="s">
         <v>125</v>
@@ -16037,7 +16043,7 @@
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B63" t="s">
         <v>113</v>
@@ -16105,7 +16111,7 @@
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B64" t="s">
         <v>104</v>
@@ -16173,7 +16179,7 @@
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B65" t="s">
         <v>92</v>
@@ -16241,7 +16247,7 @@
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B66" t="s">
         <v>60</v>
@@ -16309,7 +16315,7 @@
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B67" t="s">
         <v>97</v>
@@ -16377,7 +16383,7 @@
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B68" t="s">
         <v>134</v>
@@ -16445,7 +16451,7 @@
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B69" t="s">
         <v>58</v>
@@ -16513,7 +16519,7 @@
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B70" t="s">
         <v>73</v>
@@ -16581,7 +16587,7 @@
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B71" t="s">
         <v>122</v>
@@ -16649,7 +16655,7 @@
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B72" t="s">
         <v>114</v>
@@ -16717,7 +16723,7 @@
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B73" t="s">
         <v>78</v>
@@ -16785,7 +16791,7 @@
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B74" t="s">
         <v>106</v>
@@ -16853,7 +16859,7 @@
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B75" t="s">
         <v>77</v>
@@ -16921,7 +16927,7 @@
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B76" t="s">
         <v>95</v>
@@ -16989,7 +16995,7 @@
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B77" t="s">
         <v>124</v>
@@ -17057,7 +17063,7 @@
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B78" t="s">
         <v>127</v>
@@ -17125,7 +17131,7 @@
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B79" t="s">
         <v>99</v>
@@ -17193,7 +17199,7 @@
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B80" t="s">
         <v>108</v>

</xml_diff>